<commit_message>
Fortschritt von heute eingetragen
</commit_message>
<xml_diff>
--- a/Qalitätssicherung/TestTabelleGUI.xlsx
+++ b/Qalitätssicherung/TestTabelleGUI.xlsx
@@ -132,7 +132,7 @@
   </si>
   <si>
     <t xml:space="preserve">funktioniert, manueles eingeben von .rdbf
-Update Chiara: laden geht nicht bei &gt;2 Programmen, Eingabe wird nicht geladen</t>
+Update Chiara: laden geht wieder</t>
   </si>
   <si>
     <t xml:space="preserve">File_Menu Rest</t>
@@ -506,7 +506,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,8 +557,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFCE94F"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF73D216"/>
+        <bgColor rgb="FF92D050"/>
       </patternFill>
     </fill>
     <fill>
@@ -569,20 +569,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF73D216"/>
-        <bgColor rgb="FF92D050"/>
+        <fgColor rgb="FFD3D7CF"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFCAF3E"/>
-        <bgColor rgb="FFFFCC00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD3D7CF"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <fgColor rgb="FFFCE94F"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -690,7 +684,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -727,47 +721,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -846,7 +844,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF73D216"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFCAF3E"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF92D050"/>
@@ -868,9 +866,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -904,7 +902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="22.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -972,47 +970,47 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10" t="n">
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="n">
         <v>43156</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="n">
+      <c r="D7" s="5" t="n">
         <v>43156</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10" t="n">
+      <c r="C8" s="4"/>
+      <c r="D8" s="5" t="n">
         <v>43156</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1021,23 +1019,23 @@
       <c r="A11" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="5" t="n">
         <v>43156</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="22.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
@@ -1054,37 +1052,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="53.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="13" t="s">
+    <row r="13" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="14" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="12" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="44.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="16" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="D14" s="14" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1105,7 +1103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="22.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6" t="s">
         <v>41</v>
       </c>
@@ -1121,6 +1119,7 @@
       <c r="F16" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="M16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="6" t="s">
@@ -1140,203 +1139,203 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="10" t="n">
+      <c r="D18" s="5" t="n">
         <v>43156</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="10" t="n">
+      <c r="D20" s="5" t="n">
         <v>43156</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="10" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="5" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="5" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="19" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="10" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E23" s="11" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="5" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="10" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="D24" s="5" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="22.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="10" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E26" s="11" t="s">
+      <c r="D26" s="5" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="10" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E27" s="11" t="s">
+      <c r="D27" s="5" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="22.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="D28" s="19" t="n">
         <v>43156</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="10" t="n">
+      <c r="D29" s="5" t="n">
         <v>43156</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="10" t="n">
+      <c r="D30" s="5" t="n">
         <v>43156</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12" t="s">
+      <c r="E30" s="9"/>
+      <c r="F30" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1443,19 +1442,19 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="22.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="10" t="n">
-        <v>43158</v>
-      </c>
-      <c r="E40" s="11" t="s">
+      <c r="D40" s="5" t="n">
+        <v>43158</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1495,7 +1494,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.65"/>
   </cols>
@@ -1536,7 +1535,7 @@
       <c r="A6" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="20" t="n">
+      <c r="B6" s="21" t="n">
         <v>32.34</v>
       </c>
     </row>

</xml_diff>